<commit_message>
Ready to roll week to week
</commit_message>
<xml_diff>
--- a/data/rookierights.xlsx
+++ b/data/rookierights.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Insync/rmaxsm@umich.edu/Google Drive/FF/TRUFFLE/TRUFFLEdashGIT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57193D90-C24D-FC4F-B9A8-843D54BA72B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBAEAE2-EC94-4C41-83E2-2419AF741B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F5B89832-2916-0845-9FDE-A7E61F85B288}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{F5B89832-2916-0845-9FDE-A7E61F85B288}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>Tua Tagovailoa</t>
   </si>
@@ -60,9 +60,6 @@
     <t>JK Dobbins</t>
   </si>
   <si>
-    <t>DeAndre Swift</t>
-  </si>
-  <si>
     <t>Cam Akers</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>Chase Claypool</t>
   </si>
   <si>
-    <t>KJ Hamler</t>
-  </si>
-  <si>
     <t>Van Jefferson</t>
   </si>
   <si>
@@ -99,9 +93,6 @@
     <t>Laviska Shenault</t>
   </si>
   <si>
-    <t>Lynn Bowden</t>
-  </si>
-  <si>
     <t>Player</t>
   </si>
   <si>
@@ -180,12 +171,6 @@
     <t>Nico Collins</t>
   </si>
   <si>
-    <t>Ian Book</t>
-  </si>
-  <si>
-    <t>Dyami Brown</t>
-  </si>
-  <si>
     <t>Davis Mills</t>
   </si>
   <si>
@@ -294,13 +279,13 @@
     <t>Jelani Woods</t>
   </si>
   <si>
-    <t>Jeremy Ruckert</t>
-  </si>
-  <si>
     <t>Calvin Austin III</t>
   </si>
   <si>
     <t>Khalil Shakir</t>
+  </si>
+  <si>
+    <t>D'Andre Swift</t>
   </si>
 </sst>
 </file>
@@ -659,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB075851-A749-9F45-84CD-7B8B5DA0C6AF}">
-  <dimension ref="A1:A89"/>
+  <dimension ref="A1:A84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -672,7 +657,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -717,57 +702,57 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
@@ -777,342 +762,317 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>